<commit_message>
updated Pcollybita and Ptristis to use Ptrochillus genome, created script to run scripts 1,2,3 given species abbr as argument
</commit_message>
<xml_diff>
--- a/variant_calling_testing/_SpeciesStatus.xlsx
+++ b/variant_calling_testing/_SpeciesStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashultz/Git_Repos/comp-pop-gen/variant_calling_testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0DD1A59E-BDB6-4848-8260-1916F5268476}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C8FEBF0D-1D87-364E-B5E7-B700F0718BA2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{DA1F881D-6344-334D-AB04-9D94FA96BBB6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="18">
   <si>
     <t>Species</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Complete</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -430,7 +433,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,6 +471,9 @@
       <c r="D2" t="s">
         <v>16</v>
       </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -482,6 +488,9 @@
       <c r="D3" t="s">
         <v>16</v>
       </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -496,6 +505,9 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -510,6 +522,9 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -524,6 +539,9 @@
       <c r="D6" t="s">
         <v>16</v>
       </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -538,6 +556,9 @@
       <c r="D7" t="s">
         <v>16</v>
       </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -552,6 +573,9 @@
       <c r="D8" t="s">
         <v>16</v>
       </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -566,6 +590,9 @@
       <c r="D9" t="s">
         <v>16</v>
       </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -580,6 +607,9 @@
       <c r="D10" t="s">
         <v>16</v>
       </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -594,6 +624,9 @@
       <c r="D11" t="s">
         <v>16</v>
       </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -608,6 +641,9 @@
       <c r="D12" t="s">
         <v>16</v>
       </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -622,6 +658,9 @@
       <c r="D13" t="s">
         <v>16</v>
       </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -636,6 +675,9 @@
       <c r="D14" t="s">
         <v>16</v>
       </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -650,6 +692,9 @@
       <c r="D15" t="s">
         <v>16</v>
       </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -664,8 +709,11 @@
       <c r="D16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -678,8 +726,11 @@
       <c r="D17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -692,8 +743,11 @@
       <c r="D18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -706,8 +760,11 @@
       <c r="D19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -720,8 +777,11 @@
       <c r="D20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -734,8 +794,11 @@
       <c r="D21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -748,8 +811,11 @@
       <c r="D22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -762,8 +828,11 @@
       <c r="D23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -776,8 +845,11 @@
       <c r="D24" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -789,6 +861,9 @@
       </c>
       <c r="D25" t="s">
         <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>